<commit_message>
create 5 min cycle pie charts
</commit_message>
<xml_diff>
--- a/characteristic data/power data/benchtop_observations_feb11.xlsx
+++ b/characteristic data/power data/benchtop_observations_feb11.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SmithCA\Documents\GitHub\DHEC-Stage-Sensor\characteristic data\power data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{367B8076-66DF-4770-93D3-8A37413915DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C1AC5E-D0F4-499D-9687-8AFDA3CE6962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F7409072-B810-4EF6-94FC-057416828CA1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="50">
   <si>
     <t xml:space="preserve">Event </t>
   </si>
@@ -178,6 +178,12 @@
   </si>
   <si>
     <t>cycle with GPS consumption:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">duration with sleep: </t>
+  </si>
+  <si>
+    <t>duration no sleep:</t>
   </si>
 </sst>
 </file>
@@ -271,7 +277,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> consumption (mAH)</a:t>
+              <a:t> consumption (mAH) first cycle</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -519,7 +525,7 @@
                   <c:v>0.21777777777777776</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32388888888888889</c:v>
+                  <c:v>4.2988888888888885</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.71166666666666678</c:v>
@@ -627,7 +633,677 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>power</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> consumption (mAH) subsequent cycles</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-2A3C-480E-9EEA-BE3137E52355}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-2A3C-480E-9EEA-BE3137E52355}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-2A3C-480E-9EEA-BE3137E52355}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$83:$A$85</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>data collection (1)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>data collection (2)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sleep</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$83:$D$85</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.3888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21777777777777776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2988888888888885</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A3C-480E-9EEA-BE3137E52355}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>power consumption (mAH) with GPS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-81B0-4CFB-89E6-78AEA28F7B53}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-81B0-4CFB-89E6-78AEA28F7B53}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000004-81B0-4CFB-89E6-78AEA28F7B53}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-81B0-4CFB-89E6-78AEA28F7B53}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$83:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>data collection (1)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>data collection (2)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>sleep</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>gps</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$83:$D$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.3888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.21777777777777776</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2988888888888885</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.71166666666666678</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-81B0-4CFB-89E6-78AEA28F7B53}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1186,20 +1862,1058 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>257174</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>419099</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1219,6 +2933,78 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E08A853-E968-44D4-B521-951DCD234D75}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>300037</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5ADC1FE3-E81D-4DFF-9CD7-A37E8CB3AD17}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1524,15 +3310,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28431301-8DD6-441B-BF26-F8EECAA941AE}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:G90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="M85" sqref="M85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2100,7 +3887,7 @@
         <v>0.57444444444444442</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>13</v>
       </c>
@@ -2115,7 +3902,7 @@
         <v>0.62333333333333341</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>14</v>
       </c>
@@ -2130,7 +3917,7 @@
         <v>0.61111111111111116</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>42</v>
       </c>
@@ -2145,7 +3932,7 @@
         <v>3.3888888888888892E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>43</v>
       </c>
@@ -2160,7 +3947,7 @@
         <v>0.21777777777777776</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>16</v>
       </c>
@@ -2168,14 +3955,14 @@
         <v>53</v>
       </c>
       <c r="C85">
-        <v>22</v>
+        <v>292</v>
       </c>
       <c r="D85">
         <f t="shared" si="0"/>
-        <v>0.32388888888888889</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.2988888888888885</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -2190,7 +3977,7 @@
         <v>0.71166666666666678</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>45</v>
       </c>
@@ -2199,22 +3986,34 @@
         <v>1.808888888888889</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>46</v>
       </c>
       <c r="C89">
         <f>SUM(D83:D85)</f>
-        <v>0.5755555555555556</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>4.5505555555555555</v>
+      </c>
+      <c r="F89" t="s">
+        <v>48</v>
+      </c>
+      <c r="G89">
+        <v>2.2890000000000001</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>47</v>
       </c>
       <c r="C90">
         <f>SUM(D83:D86)</f>
-        <v>1.2872222222222223</v>
+        <v>5.2622222222222224</v>
+      </c>
+      <c r="F90" t="s">
+        <v>49</v>
+      </c>
+      <c r="G90">
+        <v>1.246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>